<commit_message>
Created functions file and implemented Pareto
Also updated Dati excel file
</commit_message>
<xml_diff>
--- a/dati_riferimento/Dati.xlsx
+++ b/dati_riferimento/Dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\OneDrive\Desktop\R\progetto\DatiRifiuti\dati_riferimento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Github\DatiMalattie\dati_riferimento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D3D825-4F4E-4A70-BB4C-550DC3BDEFAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F637AB72-8B90-4BDF-871B-BDB242234B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40320" yWindow="4380" windowWidth="17280" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10725" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Rifiuti organici</t>
   </si>
@@ -43,6 +43,93 @@
   </si>
   <si>
     <t>Altro</t>
+  </si>
+  <si>
+    <t>Piemonte</t>
+  </si>
+  <si>
+    <t>Valle d'Aosta /Vallée d'Aoste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liguria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lombardia  </t>
+  </si>
+  <si>
+    <t>Trentino-Alto Adige/Südtirol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolzano-Bozen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veneto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friuli-Venezia Giulia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilia-Romagna </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toscana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umbria </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marche </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lazio </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abruzzo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campania </t>
+  </si>
+  <si>
+    <t>Puglia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basilicata </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calabria </t>
+  </si>
+  <si>
+    <t>Sicilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sardegna </t>
+  </si>
+  <si>
+    <t>Nord-ovest</t>
+  </si>
+  <si>
+    <t>Nord-est</t>
+  </si>
+  <si>
+    <t>Centro</t>
+  </si>
+  <si>
+    <t>Sud</t>
+  </si>
+  <si>
+    <t>Isole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITALIA </t>
+  </si>
+  <si>
+    <t>Regioni</t>
   </si>
 </sst>
 </file>
@@ -101,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -114,6 +201,15 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -396,591 +492,678 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
         <v>840807.28599999996</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>409526.74599999998</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>265958.788</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>160677.50700000001</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>125039.088</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>261571.747</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
         <v>28649.15</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>14581.43</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>9387.06</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>6684.81</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>6159.85</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>8259.1489999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
         <v>424884.16200000001</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>128256.933</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>84428.176999999996</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>60408.302000000003</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>33569.406999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>98488.743999999992</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1">
         <v>1423822.156</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>1206022.801</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>546998.66200000001</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>422743.86599999998</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>248268.28700000001</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>837632.95400000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
         <v>147532.68700000001</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
         <v>133535.46100000001</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>83541.5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>43738.559000000001</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>33093.294999999998</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>77592.393000000011</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
         <v>81059.948999999993</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>60819.942000000003</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>42239.466999999997</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>25372.530999999999</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>8520.2049999999999</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>39637.826999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
         <v>66472.737999999998</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>72715.519</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>41302.033000000003</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>18366.027999999998</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>24573.089</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>37954.563999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
         <v>615317.16599999997</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>764526.326</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>286931.39799999999</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>222674.47</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>117035.75599999999</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>328308.62099999998</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1">
         <v>203354.28200000001</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>166913.20199999999</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>68954.301000000007</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>45152.906999999999</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>26347.534</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>78295.808000000005</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
         <v>1034390.547</v>
       </c>
-      <c r="B11" s="1">
+      <c r="C11" s="1">
         <v>708243.51500000001</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>385188.05800000002</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>160641.61499999999</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>137038.13800000001</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>434261.50000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1">
         <v>1034845.95</v>
       </c>
-      <c r="B12" s="1">
+      <c r="C12" s="1">
         <v>494221.74300000002</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>283163.33899999998</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>116695.05100000001</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>85732.006999999998</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>229162.21200000003</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="1">
         <v>172705.73200000002</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>116919.401</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>57202.076999999997</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>27105.895</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>22719.424999999999</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>54177.954000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
         <v>300266.40899999999</v>
       </c>
-      <c r="B14" s="1">
+      <c r="C14" s="1">
         <v>232083.522</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>111477.728</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>61059.19</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>24787.602999999999</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>87309.756000000008</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
         <v>1607960.8149999999</v>
       </c>
-      <c r="B15" s="1">
+      <c r="C15" s="1">
         <v>532659.35600000003</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>346594.25</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>212490.55</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>73530.09</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>188631.68799999985</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1">
         <v>262623.80600000004</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>149314.06</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>77083.039000000004</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>49747.016000000003</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>15088.096</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>42888.524000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
         <v>80819.482000000004</v>
       </c>
-      <c r="B17" s="1">
+      <c r="C17" s="1">
         <v>14953.401</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>6802.491</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>6672.2950000000001</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>4156.8010000000004</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>3253.3249999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1">
         <v>1209746.6810000001</v>
       </c>
-      <c r="B18" s="1">
+      <c r="C18" s="1">
         <v>678908.04599999997</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>180334.677</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>136738.16399999999</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>137860.20300000001</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>217410.76699999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="1">
         <v>1117599.564</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>291501.24</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>177167.647</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>82466.895000000004</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>75583.899999999994</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>132015.86499999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1">
         <v>107409.01999999999</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>31233.745999999999</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>23203.205000000002</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>12332.278</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>7446.8289999999997</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>14689.986999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
         <v>466847.00299999997</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>126579.81299999999</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>76407.718999999997</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>45004.35</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>16489.052</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>42461.591</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1">
         <v>1800509.1410000001</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>208309.14120000001</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>123274.322</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>56830.928</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>38333.347999999998</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>72939.117800000007</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1">
         <v>267312.446</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>213663.386</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>83011.918000000005</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>70519.119000000006</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>45376.038</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>43589.554999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4">
         <v>2718162.7539999997</v>
       </c>
-      <c r="B24" s="4">
+      <c r="C24" s="4">
         <v>1758387.91</v>
       </c>
-      <c r="C24" s="4">
+      <c r="D24" s="4">
         <v>906772.68700000003</v>
       </c>
-      <c r="D24" s="4">
+      <c r="E24" s="4">
         <v>650514.48499999999</v>
       </c>
-      <c r="E24" s="4">
+      <c r="F24" s="4">
         <v>413036.63199999998</v>
       </c>
-      <c r="F24" s="4">
+      <c r="G24" s="4">
         <v>1205952.594</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="4">
         <v>2000594.682</v>
       </c>
-      <c r="B25" s="4">
+      <c r="C25" s="4">
         <v>1773218.5040000002</v>
       </c>
-      <c r="C25" s="4">
+      <c r="D25" s="4">
         <v>824615.25699999998</v>
       </c>
-      <c r="D25" s="4">
+      <c r="E25" s="4">
         <v>472207.55099999998</v>
       </c>
-      <c r="E25" s="4">
+      <c r="F25" s="4">
         <v>313514.72199999995</v>
       </c>
-      <c r="F25" s="4">
+      <c r="G25" s="4">
         <v>918458.32000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="4">
         <v>3115778.906</v>
       </c>
-      <c r="B26" s="4">
+      <c r="C26" s="4">
         <v>1375884.0219999999</v>
       </c>
-      <c r="C26" s="4">
+      <c r="D26" s="4">
         <v>798437.39399999997</v>
       </c>
-      <c r="D26" s="4">
+      <c r="E26" s="4">
         <v>417350.68599999999</v>
       </c>
-      <c r="E26" s="4">
+      <c r="F26" s="4">
         <v>206769.125</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
         <v>559281.60999999987</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="4">
         <v>3245045.5559999999</v>
       </c>
-      <c r="B27" s="4">
+      <c r="C27" s="4">
         <v>1292490.3060000001</v>
       </c>
-      <c r="C27" s="4">
+      <c r="D27" s="4">
         <v>540998.77800000005</v>
       </c>
-      <c r="D27" s="4">
+      <c r="E27" s="4">
         <v>332960.99799999996</v>
       </c>
-      <c r="E27" s="4">
+      <c r="F27" s="4">
         <v>256624.88099999999</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
         <v>452720.05900000001</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="4">
         <v>2067821.5870000001</v>
       </c>
-      <c r="B28" s="4">
+      <c r="C28" s="4">
         <v>421972.52720000001</v>
       </c>
-      <c r="C28" s="4">
+      <c r="D28" s="4">
         <v>206286.24</v>
       </c>
-      <c r="D28" s="4">
+      <c r="E28" s="4">
         <v>127350.04700000001</v>
       </c>
-      <c r="E28" s="4">
+      <c r="F28" s="4">
         <v>83709.385999999999</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
         <v>116528.6728</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="4">
         <v>13147403.484999999</v>
       </c>
-      <c r="B29" s="4">
+      <c r="C29" s="4">
         <v>6621953.2692</v>
       </c>
-      <c r="C29" s="4">
+      <c r="D29" s="4">
         <v>3277110.3559999997</v>
       </c>
-      <c r="D29" s="4">
+      <c r="E29" s="4">
         <v>2000383.7669999998</v>
       </c>
-      <c r="E29" s="4">
+      <c r="F29" s="4">
         <v>1273654.7459999998</v>
       </c>
-      <c r="F29" s="4">
+      <c r="G29" s="4">
         <v>3252941.2557999995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed Trento and Bolzano
</commit_message>
<xml_diff>
--- a/dati_riferimento/Dati.xlsx
+++ b/dati_riferimento/Dati.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\OneDrive\Documenti\GitHub\DatiRifiuti\dati_riferimento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DatiRifiuti\dati_riferimento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7B7561-9953-4117-8617-16BF32A443C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66D88A8-1020-4DCD-A6EC-567C50D51020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40320" yWindow="4380" windowWidth="17280" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Rifiuti organici</t>
   </si>
@@ -58,12 +58,6 @@
   </si>
   <si>
     <t>Trentino-Alto Adige/Südtirol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bolzano-Bozen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trento </t>
   </si>
   <si>
     <t xml:space="preserve">Veneto </t>
@@ -118,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,12 +126,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="7"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -164,21 +152,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,17 +441,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -493,8 +472,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1">
@@ -516,8 +495,8 @@
         <v>261571.747</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1">
@@ -539,8 +518,8 @@
         <v>8259.1489999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
@@ -562,8 +541,8 @@
         <v>98488.743999999992</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1">
@@ -585,8 +564,8 @@
         <v>837632.95400000003</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1">
@@ -608,394 +587,348 @@
         <v>77592.393000000011</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
-        <v>81059.948999999993</v>
-      </c>
-      <c r="C7" s="3">
-        <v>60819.942000000003</v>
-      </c>
-      <c r="D7" s="3">
-        <v>42239.466999999997</v>
-      </c>
-      <c r="E7" s="3">
-        <v>25372.530999999999</v>
-      </c>
-      <c r="F7" s="3">
-        <v>8520.2049999999999</v>
-      </c>
-      <c r="G7" s="3">
-        <v>39637.826999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="B7" s="1">
+        <v>615317.16599999997</v>
+      </c>
+      <c r="C7" s="1">
+        <v>764526.326</v>
+      </c>
+      <c r="D7" s="1">
+        <v>286931.39799999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>222674.47</v>
+      </c>
+      <c r="F7" s="1">
+        <v>117035.75599999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>328308.62099999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
-        <v>66472.737999999998</v>
-      </c>
-      <c r="C8" s="3">
-        <v>72715.519</v>
-      </c>
-      <c r="D8" s="3">
-        <v>41302.033000000003</v>
-      </c>
-      <c r="E8" s="3">
-        <v>18366.027999999998</v>
-      </c>
-      <c r="F8" s="3">
-        <v>24573.089</v>
-      </c>
-      <c r="G8" s="3">
-        <v>37954.563999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B8" s="1">
+        <v>203354.28200000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>166913.20199999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>68954.301000000007</v>
+      </c>
+      <c r="E8" s="1">
+        <v>45152.906999999999</v>
+      </c>
+      <c r="F8" s="1">
+        <v>26347.534</v>
+      </c>
+      <c r="G8" s="1">
+        <v>78295.808000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="1">
-        <v>615317.16599999997</v>
+        <v>1034390.547</v>
       </c>
       <c r="C9" s="1">
-        <v>764526.326</v>
+        <v>708243.51500000001</v>
       </c>
       <c r="D9" s="1">
-        <v>286931.39799999999</v>
+        <v>385188.05800000002</v>
       </c>
       <c r="E9" s="1">
-        <v>222674.47</v>
+        <v>160641.61499999999</v>
       </c>
       <c r="F9" s="1">
-        <v>117035.75599999999</v>
+        <v>137038.13800000001</v>
       </c>
       <c r="G9" s="1">
-        <v>328308.62099999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+        <v>434261.50000000006</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1">
-        <v>203354.28200000001</v>
+        <v>1034845.95</v>
       </c>
       <c r="C10" s="1">
-        <v>166913.20199999999</v>
+        <v>494221.74300000002</v>
       </c>
       <c r="D10" s="1">
-        <v>68954.301000000007</v>
+        <v>283163.33899999998</v>
       </c>
       <c r="E10" s="1">
-        <v>45152.906999999999</v>
+        <v>116695.05100000001</v>
       </c>
       <c r="F10" s="1">
-        <v>26347.534</v>
+        <v>85732.006999999998</v>
       </c>
       <c r="G10" s="1">
-        <v>78295.808000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+        <v>229162.21200000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="1">
-        <v>1034390.547</v>
+        <v>172705.73200000002</v>
       </c>
       <c r="C11" s="1">
-        <v>708243.51500000001</v>
+        <v>116919.401</v>
       </c>
       <c r="D11" s="1">
-        <v>385188.05800000002</v>
+        <v>57202.076999999997</v>
       </c>
       <c r="E11" s="1">
-        <v>160641.61499999999</v>
+        <v>27105.895</v>
       </c>
       <c r="F11" s="1">
-        <v>137038.13800000001</v>
+        <v>22719.424999999999</v>
       </c>
       <c r="G11" s="1">
-        <v>434261.50000000006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+        <v>54177.954000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>1034845.95</v>
+        <v>300266.40899999999</v>
       </c>
       <c r="C12" s="1">
-        <v>494221.74300000002</v>
+        <v>232083.522</v>
       </c>
       <c r="D12" s="1">
-        <v>283163.33899999998</v>
+        <v>111477.728</v>
       </c>
       <c r="E12" s="1">
-        <v>116695.05100000001</v>
+        <v>61059.19</v>
       </c>
       <c r="F12" s="1">
-        <v>85732.006999999998</v>
+        <v>24787.602999999999</v>
       </c>
       <c r="G12" s="1">
-        <v>229162.21200000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+        <v>87309.756000000008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1">
-        <v>172705.73200000002</v>
+        <v>1607960.8149999999</v>
       </c>
       <c r="C13" s="1">
-        <v>116919.401</v>
+        <v>532659.35600000003</v>
       </c>
       <c r="D13" s="1">
-        <v>57202.076999999997</v>
+        <v>346594.25</v>
       </c>
       <c r="E13" s="1">
-        <v>27105.895</v>
+        <v>212490.55</v>
       </c>
       <c r="F13" s="1">
-        <v>22719.424999999999</v>
+        <v>73530.09</v>
       </c>
       <c r="G13" s="1">
-        <v>54177.954000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+        <v>188631.68799999985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="1">
-        <v>300266.40899999999</v>
+        <v>262623.80600000004</v>
       </c>
       <c r="C14" s="1">
-        <v>232083.522</v>
+        <v>149314.06</v>
       </c>
       <c r="D14" s="1">
-        <v>111477.728</v>
+        <v>77083.039000000004</v>
       </c>
       <c r="E14" s="1">
-        <v>61059.19</v>
+        <v>49747.016000000003</v>
       </c>
       <c r="F14" s="1">
-        <v>24787.602999999999</v>
+        <v>15088.096</v>
       </c>
       <c r="G14" s="1">
-        <v>87309.756000000008</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+        <v>42888.524000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B15" s="1">
-        <v>1607960.8149999999</v>
+        <v>80819.482000000004</v>
       </c>
       <c r="C15" s="1">
-        <v>532659.35600000003</v>
+        <v>14953.401</v>
       </c>
       <c r="D15" s="1">
-        <v>346594.25</v>
+        <v>6802.491</v>
       </c>
       <c r="E15" s="1">
-        <v>212490.55</v>
+        <v>6672.2950000000001</v>
       </c>
       <c r="F15" s="1">
-        <v>73530.09</v>
+        <v>4156.8010000000004</v>
       </c>
       <c r="G15" s="1">
-        <v>188631.68799999985</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+        <v>3253.3249999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="1">
-        <v>262623.80600000004</v>
+        <v>1209746.6810000001</v>
       </c>
       <c r="C16" s="1">
-        <v>149314.06</v>
+        <v>678908.04599999997</v>
       </c>
       <c r="D16" s="1">
-        <v>77083.039000000004</v>
+        <v>180334.677</v>
       </c>
       <c r="E16" s="1">
-        <v>49747.016000000003</v>
+        <v>136738.16399999999</v>
       </c>
       <c r="F16" s="1">
-        <v>15088.096</v>
+        <v>137860.20300000001</v>
       </c>
       <c r="G16" s="1">
-        <v>42888.524000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+        <v>217410.76699999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="1">
-        <v>80819.482000000004</v>
+        <v>1117599.564</v>
       </c>
       <c r="C17" s="1">
-        <v>14953.401</v>
+        <v>291501.24</v>
       </c>
       <c r="D17" s="1">
-        <v>6802.491</v>
+        <v>177167.647</v>
       </c>
       <c r="E17" s="1">
-        <v>6672.2950000000001</v>
+        <v>82466.895000000004</v>
       </c>
       <c r="F17" s="1">
-        <v>4156.8010000000004</v>
+        <v>75583.899999999994</v>
       </c>
       <c r="G17" s="1">
-        <v>3253.3249999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+        <v>132015.86499999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="1">
-        <v>1209746.6810000001</v>
+        <v>107409.01999999999</v>
       </c>
       <c r="C18" s="1">
-        <v>678908.04599999997</v>
+        <v>31233.745999999999</v>
       </c>
       <c r="D18" s="1">
-        <v>180334.677</v>
+        <v>23203.205000000002</v>
       </c>
       <c r="E18" s="1">
-        <v>136738.16399999999</v>
+        <v>12332.278</v>
       </c>
       <c r="F18" s="1">
-        <v>137860.20300000001</v>
+        <v>7446.8289999999997</v>
       </c>
       <c r="G18" s="1">
-        <v>217410.76699999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+        <v>14689.986999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="1">
-        <v>1117599.564</v>
+        <v>466847.00299999997</v>
       </c>
       <c r="C19" s="1">
-        <v>291501.24</v>
+        <v>126579.81299999999</v>
       </c>
       <c r="D19" s="1">
-        <v>177167.647</v>
+        <v>76407.718999999997</v>
       </c>
       <c r="E19" s="1">
-        <v>82466.895000000004</v>
+        <v>45004.35</v>
       </c>
       <c r="F19" s="1">
-        <v>75583.899999999994</v>
+        <v>16489.052</v>
       </c>
       <c r="G19" s="1">
-        <v>132015.86499999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+        <v>42461.591</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1">
-        <v>107409.01999999999</v>
+        <v>1800509.1410000001</v>
       </c>
       <c r="C20" s="1">
-        <v>31233.745999999999</v>
+        <v>208309.14120000001</v>
       </c>
       <c r="D20" s="1">
-        <v>23203.205000000002</v>
+        <v>123274.322</v>
       </c>
       <c r="E20" s="1">
-        <v>12332.278</v>
+        <v>56830.928</v>
       </c>
       <c r="F20" s="1">
-        <v>7446.8289999999997</v>
+        <v>38333.347999999998</v>
       </c>
       <c r="G20" s="1">
-        <v>14689.986999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+        <v>72939.117800000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1">
-        <v>466847.00299999997</v>
+        <v>267312.446</v>
       </c>
       <c r="C21" s="1">
-        <v>126579.81299999999</v>
+        <v>213663.386</v>
       </c>
       <c r="D21" s="1">
-        <v>76407.718999999997</v>
+        <v>83011.918000000005</v>
       </c>
       <c r="E21" s="1">
-        <v>45004.35</v>
+        <v>70519.119000000006</v>
       </c>
       <c r="F21" s="1">
-        <v>16489.052</v>
+        <v>45376.038</v>
       </c>
       <c r="G21" s="1">
-        <v>42461.591</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1800509.1410000001</v>
-      </c>
-      <c r="C22" s="1">
-        <v>208309.14120000001</v>
-      </c>
-      <c r="D22" s="1">
-        <v>123274.322</v>
-      </c>
-      <c r="E22" s="1">
-        <v>56830.928</v>
-      </c>
-      <c r="F22" s="1">
-        <v>38333.347999999998</v>
-      </c>
-      <c r="G22" s="1">
-        <v>72939.117800000007</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="1">
-        <v>267312.446</v>
-      </c>
-      <c r="C23" s="1">
-        <v>213663.386</v>
-      </c>
-      <c r="D23" s="1">
-        <v>83011.918000000005</v>
-      </c>
-      <c r="E23" s="1">
-        <v>70519.119000000006</v>
-      </c>
-      <c r="F23" s="1">
-        <v>45376.038</v>
-      </c>
-      <c r="G23" s="1">
         <v>43589.554999999993</v>
       </c>
     </row>

</xml_diff>